<commit_message>
fix: number type in output excel
</commit_message>
<xml_diff>
--- a/model_evaluation.xlsx
+++ b/model_evaluation.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Evaluasi" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -18,18 +18,15 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -40,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -48,22 +45,14 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -438,87 +427,87 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Tanggal_Update</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>RMSE</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>MAPE</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>R2</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>MSE</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Jumlah_Data_Evaluasi</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>MSE_Price</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>RMSE_Price</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>MAE_Price</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>R2_Price</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n">
-        <v>45936</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0.008047985414953484</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1.149062054539716</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.06336290163663183</v>
-      </c>
-      <c r="E2" t="n">
-        <v>6.477006923930401e-05</v>
-      </c>
-      <c r="F2" t="n">
+      <c r="A2" s="1" t="n">
+        <v>45937</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>0.008217311197419652</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>1.465681849318622</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>0.01215766150392072</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>6.75242033152384e-05</v>
+      </c>
+      <c r="F2" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="G2" t="n">
-        <v>4097.941492097407</v>
-      </c>
-      <c r="H2" t="n">
-        <v>64.01516611005088</v>
-      </c>
-      <c r="I2" t="n">
-        <v>52.99226145623734</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0.7872505150469828</v>
+      <c r="G2" s="2" t="n">
+        <v>4277.950583559414</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>65.40604393754001</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>54.02125274057797</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>0.7915770596779452</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: number formatting in gsheet
</commit_message>
<xml_diff>
--- a/model_evaluation.xlsx
+++ b/model_evaluation.xlsx
@@ -16,9 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="165" formatCode="[$-421]#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -51,8 +52,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>

</xml_diff>

<commit_message>
fix: only update new data in gsheet, update start date to 1993 on fetching yfinance data
</commit_message>
<xml_diff>
--- a/model_evaluation.xlsx
+++ b/model_evaluation.xlsx
@@ -481,34 +481,34 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>45937</v>
+        <v>45944</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.008217311197419652</v>
+        <v>0.007679953205691472</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>1.465681849318622</v>
+        <v>1.626911367747524</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>0.01215766150392072</v>
+        <v>0.02282632902275583</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>6.75242033152384e-05</v>
+        <v>5.898168124161073e-05</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>29</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>4277.950583559414</v>
+        <v>3492.988802624848</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>65.40604393754001</v>
+        <v>59.10151269320311</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>54.02125274057797</v>
+        <v>49.10089788410074</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>0.7915770596779452</v>
+        <v>0.8710329042982154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: solve issuses about model evaluation sheet not being updated
</commit_message>
<xml_diff>
--- a/model_evaluation.xlsx
+++ b/model_evaluation.xlsx
@@ -481,34 +481,34 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>45944</v>
+        <v>45949</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.007679953205691472</v>
+        <v>0.009329675380027286</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>1.626911367747524</v>
+        <v>1.610176344153507</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>0.02282632902275583</v>
+        <v>0.02747964137393155</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>5.898168124161073e-05</v>
+        <v>8.704284269668728e-05</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>29</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>3492.988802624848</v>
+        <v>5481.429871186317</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>59.10151269320311</v>
+        <v>74.03667922851697</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>49.10089788410074</v>
+        <v>55.92120153249586</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>0.8710329042982154</v>
+        <v>0.7554013296252071</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: actual and prediction column, remove status column
</commit_message>
<xml_diff>
--- a/model_evaluation.xlsx
+++ b/model_evaluation.xlsx
@@ -481,34 +481,34 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>45954</v>
+        <v>45956</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.01023721997442861</v>
+        <v>0.009966437180098865</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>1.617026993680357</v>
+        <v>1.77646509386</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>-0.02064236629879224</v>
+        <v>-0.01040491458725823</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>0.0001048006728048401</v>
+        <v>9.9329870064857e-05</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>29</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>6721.437483416983</v>
+        <v>6559.115053537917</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>81.98437340991869</v>
+        <v>80.98836369218677</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>61.88505157790396</v>
+        <v>59.98225770763258</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>0.1977963765610751</v>
+        <v>0.2103258227616113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: evalation based on last 30 days data
</commit_message>
<xml_diff>
--- a/model_evaluation.xlsx
+++ b/model_evaluation.xlsx
@@ -18,8 +18,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="165" formatCode="[$-421]#,##0.00"/>
-    <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="[$-421]#,##0.00"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -50,10 +50,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -484,31 +485,31 @@
         <v>45961</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.01042322294647325</v>
+        <v>0.005080933345529242</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>1.754400925969261</v>
+        <v>0.9057459357033854</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>0.005348041151770344</v>
+        <v>0.8129863656775127</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>0.0001086435765918865</v>
-      </c>
-      <c r="F2" s="2" t="n">
-        <v>29</v>
+        <v>2.581588366171098e-05</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>21</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>7367.358665391402</v>
+        <v>1749.95412525557</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>85.83331908642123</v>
+        <v>41.83245301504049</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>64.12873118220435</v>
+        <v>21.63134065291425</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>-0.1069589500099655</v>
+        <v>0.7638187495916015</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: value in Jumlah_Data_Evaluasi evaluation sheet
</commit_message>
<xml_diff>
--- a/model_evaluation.xlsx
+++ b/model_evaluation.xlsx
@@ -485,31 +485,31 @@
         <v>45965</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.005375553564523805</v>
+        <v>0.00516220261919316</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>1.009767505000193</v>
+        <v>1.374451949963991</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>0.8085599273152317</v>
+        <v>0.767956424923307</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>2.889657612506459e-05</v>
+        <v>2.664833588160472e-05</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>1959.218308016009</v>
+        <v>1796.206321674443</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>44.26305805088493</v>
+        <v>42.38167436138458</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>23.45915804915273</v>
+        <v>24.32737954491605</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>0.7477612869159103</v>
+        <v>0.7444787810482614</v>
       </c>
     </row>
   </sheetData>

</xml_diff>